<commit_message>
Getting Basics In Place, A Map and Pulling Data From Db to View
</commit_message>
<xml_diff>
--- a/dataAboutCities.xlsx
+++ b/dataAboutCities.xlsx
@@ -1024,7 +1024,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1059,7 +1059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F297"/>
+  <dimension ref="A1:H297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1355,7 +1355,7 @@
     <col min="6" max="6" width="8.81640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1374,8 +1374,12 @@
       <c r="F1" s="3">
         <v>73.938500000000005</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="1">
+        <f>MAX(D:D)</f>
+        <v>1704.7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1394,8 +1398,12 @@
       <c r="F2" s="3">
         <v>118.41079999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2" s="3">
+        <f>MAX(E:E)</f>
+        <v>61.217599999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1414,8 +1422,12 @@
       <c r="F3" s="3">
         <v>87.681799999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H3" s="3">
+        <f>MAX(F:F)</f>
+        <v>157.84530000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -1435,7 +1447,7 @@
         <v>95.386300000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>75.133300000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1487,7 @@
         <v>112.08799999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>98.525099999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1515,7 +1527,7 @@
         <v>117.13500000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>96.796700000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1555,7 +1567,7 @@
         <v>121.8193</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1575,7 +1587,7 @@
         <v>97.756</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>301</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>81.661299999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>302</v>
       </c>
@@ -1615,7 +1627,7 @@
         <v>122.41930000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>303</v>
       </c>
@@ -1635,7 +1647,7 @@
         <v>86.145899999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1655,7 +1667,7 @@
         <v>82.984999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>